<commit_message>
Updated Convergence History Process
</commit_message>
<xml_diff>
--- a/Base Case Solution.xlsx
+++ b/Base Case Solution.xlsx
@@ -1175,7 +1175,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1229,6 +1229,23 @@
         <v>0.04502560403869005</v>
       </c>
       <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.0001561433034621418</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.0001598378424807478</v>
+      </c>
+      <c r="E4">
         <v>5</v>
       </c>
     </row>

</xml_diff>